<commit_message>
Changed name of cluster
</commit_message>
<xml_diff>
--- a/projects/NECB_All_Buildings_Vancouver_Baseline_Test.xlsx
+++ b/projects/NECB_All_Buildings_Vancouver_Baseline_Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5310" windowWidth="20370" windowHeight="5205" tabRatio="469" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="5310" windowWidth="20370" windowHeight="5205" tabRatio="469" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -722,12 +722,6 @@
     <t>ft^2*h*R/Btu</t>
   </si>
   <si>
-    <t>aparker</t>
-  </si>
-  <si>
-    <t>Ptool_Full_Analysis</t>
-  </si>
-  <si>
     <t>Roof Insulation</t>
   </si>
   <si>
@@ -746,9 +740,6 @@
     <t>delta_x</t>
   </si>
   <si>
-    <t>PToolFullCluster</t>
-  </si>
-  <si>
     <t>MediumOffice</t>
   </si>
   <si>
@@ -1509,6 +1500,15 @@
   </si>
   <si>
     <t>ReportingMeasure</t>
+  </si>
+  <si>
+    <t>Phylroy-NECB Analysis</t>
+  </si>
+  <si>
+    <t>Phylroys_Cluster</t>
+  </si>
+  <si>
+    <t>plopez</t>
   </si>
 </sst>
 </file>
@@ -6360,8 +6360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6408,7 +6408,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>228</v>
+        <v>490</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>69</v>
@@ -6419,7 +6419,7 @@
         <v>79</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>162</v>
@@ -6430,7 +6430,7 @@
         <v>80</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>236</v>
+        <v>489</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>82</v>
@@ -6501,7 +6501,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>229</v>
+        <v>488</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>81</v>
@@ -6699,7 +6699,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -6707,7 +6707,7 @@
         <v>27</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C37" s="29"/>
     </row>
@@ -6716,7 +6716,7 @@
         <v>27</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D38" s="2"/>
     </row>
@@ -6725,7 +6725,7 @@
         <v>27</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D39" s="2"/>
     </row>
@@ -6734,7 +6734,7 @@
         <v>27</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D40" s="2"/>
     </row>
@@ -6763,7 +6763,7 @@
         <v>180</v>
       </c>
       <c r="D43" s="29" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>200</v>
@@ -6818,8 +6818,8 @@
   </sheetPr>
   <dimension ref="A1:Z16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -6944,7 +6944,7 @@
         <v>8</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="P3" s="16" t="s">
         <v>85</v>
@@ -7011,25 +7011,25 @@
         <v>209</v>
       </c>
       <c r="I5" s="58" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="J5" s="75" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="K5" s="58" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L5" s="58" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="M5" s="58" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N5" s="58" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="P5" s="58" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="R5" s="58" t="s">
         <v>216</v>
@@ -7050,25 +7050,25 @@
         <v>209</v>
       </c>
       <c r="I6" s="58" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="J6" s="58" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K6" s="58" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="L6" s="58" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="M6" s="58" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="N6" s="58" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="P6" s="58" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="R6" s="58" t="s">
         <v>216</v>
@@ -7089,25 +7089,25 @@
         <v>209</v>
       </c>
       <c r="I7" s="59" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="J7" s="58" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K7" s="59" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L7" s="59" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="M7" s="59" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="N7" s="59" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="P7" s="59" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="R7" s="58" t="s">
         <v>216</v>
@@ -7119,34 +7119,34 @@
         <v>221</v>
       </c>
       <c r="D8" s="58" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E8" s="58" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G8" s="58" t="s">
         <v>209</v>
       </c>
       <c r="I8" s="59" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J8" s="58" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K8" s="59" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="L8" s="59" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M8" s="59" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N8" s="59" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="P8" s="59" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="R8" s="58" t="s">
         <v>216</v>
@@ -7157,13 +7157,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="67" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D9" s="62" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E9" s="62" t="s">
         <v>45</v>
@@ -7217,7 +7217,7 @@
         <v>226</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>43</v>
@@ -7235,13 +7235,13 @@
         <v>1</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E12" s="64" t="s">
         <v>45</v>
@@ -7258,36 +7258,36 @@
         <v>20</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F13" s="53"/>
       <c r="G13" s="53" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H13" s="53"/>
       <c r="I13" s="55" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="J13" s="53" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="K13" s="54" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="L13" s="54" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="M13" s="54" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="N13" s="54" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="P13" s="54" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="R13" s="54" t="s">
         <v>216</v>
@@ -7299,24 +7299,24 @@
         <v>20</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E14" s="53" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="F14" s="53"/>
       <c r="G14" s="53" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H14" s="53"/>
       <c r="I14" s="53" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J14" s="53" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="P14" s="54" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="R14" s="54" t="s">
         <v>216</v>
@@ -7327,16 +7327,16 @@
         <v>1</v>
       </c>
       <c r="B15" s="57" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C15" s="57" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="D15" s="57" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="E15" s="57" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="I15" s="51"/>
       <c r="J15" s="51"/>
@@ -7346,16 +7346,16 @@
         <v>1</v>
       </c>
       <c r="B16" s="78" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C16" s="78" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D16" s="78" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="E16" s="55" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="I16" s="79"/>
       <c r="J16" s="79"/>
@@ -7375,7 +7375,7 @@
   <dimension ref="A1:M197"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B205" sqref="B205"/>
     </sheetView>
   </sheetViews>
@@ -7968,10 +7968,10 @@
     </row>
     <row r="21" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="G21" s="77" t="b">
         <v>1</v>
@@ -7985,10 +7985,10 @@
     </row>
     <row r="22" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="G22" s="77" t="b">
         <v>1</v>
@@ -8002,10 +8002,10 @@
     </row>
     <row r="23" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G23" s="77" t="b">
         <v>1</v>
@@ -8019,10 +8019,10 @@
     </row>
     <row r="24" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="G24" s="77" t="b">
         <v>1</v>
@@ -8036,10 +8036,10 @@
     </row>
     <row r="25" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G25" s="77" t="b">
         <v>1</v>
@@ -8053,10 +8053,10 @@
     </row>
     <row r="26" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G26" s="77" t="b">
         <v>1</v>
@@ -8070,10 +8070,10 @@
     </row>
     <row r="27" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="G27" s="77" t="b">
         <v>1</v>
@@ -8087,10 +8087,10 @@
     </row>
     <row r="28" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G28" s="77" t="b">
         <v>1</v>
@@ -8104,10 +8104,10 @@
     </row>
     <row r="29" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G29" s="77" t="b">
         <v>1</v>
@@ -8121,10 +8121,10 @@
     </row>
     <row r="30" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G30" s="77" t="b">
         <v>1</v>
@@ -8138,10 +8138,10 @@
     </row>
     <row r="31" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G31" s="77" t="b">
         <v>1</v>
@@ -8155,10 +8155,10 @@
     </row>
     <row r="32" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G32" s="77" t="b">
         <v>1</v>
@@ -8172,10 +8172,10 @@
     </row>
     <row r="33" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G33" s="77" t="b">
         <v>1</v>
@@ -8189,10 +8189,10 @@
     </row>
     <row r="34" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G34" s="77" t="b">
         <v>1</v>
@@ -8206,10 +8206,10 @@
     </row>
     <row r="35" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D35" s="18" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G35" s="77" t="b">
         <v>1</v>
@@ -8223,10 +8223,10 @@
     </row>
     <row r="36" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G36" s="77" t="b">
         <v>1</v>
@@ -8240,10 +8240,10 @@
     </row>
     <row r="37" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G37" s="77" t="b">
         <v>1</v>
@@ -8257,10 +8257,10 @@
     </row>
     <row r="38" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G38" s="77" t="b">
         <v>1</v>
@@ -8274,10 +8274,10 @@
     </row>
     <row r="39" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G39" s="77" t="b">
         <v>1</v>
@@ -8291,10 +8291,10 @@
     </row>
     <row r="40" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G40" s="77" t="b">
         <v>1</v>
@@ -8308,10 +8308,10 @@
     </row>
     <row r="41" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G41" s="77" t="b">
         <v>1</v>
@@ -8325,10 +8325,10 @@
     </row>
     <row r="42" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G42" s="77" t="b">
         <v>1</v>
@@ -8342,10 +8342,10 @@
     </row>
     <row r="43" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G43" s="77" t="b">
         <v>1</v>
@@ -8359,10 +8359,10 @@
     </row>
     <row r="44" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G44" s="77" t="b">
         <v>1</v>
@@ -8376,10 +8376,10 @@
     </row>
     <row r="45" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G45" s="77" t="b">
         <v>1</v>
@@ -8393,10 +8393,10 @@
     </row>
     <row r="46" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G46" s="77" t="b">
         <v>1</v>
@@ -8410,10 +8410,10 @@
     </row>
     <row r="47" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G47" s="77" t="b">
         <v>1</v>
@@ -8427,10 +8427,10 @@
     </row>
     <row r="48" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G48" s="77" t="b">
         <v>1</v>
@@ -8444,10 +8444,10 @@
     </row>
     <row r="49" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G49" s="77" t="b">
         <v>1</v>
@@ -8461,10 +8461,10 @@
     </row>
     <row r="50" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G50" s="77" t="b">
         <v>1</v>
@@ -8478,10 +8478,10 @@
     </row>
     <row r="51" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="G51" s="77" t="b">
         <v>1</v>
@@ -8495,10 +8495,10 @@
     </row>
     <row r="52" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G52" s="77" t="b">
         <v>1</v>
@@ -8512,10 +8512,10 @@
     </row>
     <row r="53" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="18" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="G53" s="77" t="b">
         <v>1</v>
@@ -8529,10 +8529,10 @@
     </row>
     <row r="54" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="18" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="G54" s="77" t="b">
         <v>1</v>
@@ -8546,10 +8546,10 @@
     </row>
     <row r="55" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G55" s="77" t="b">
         <v>1</v>
@@ -8563,10 +8563,10 @@
     </row>
     <row r="56" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="G56" s="77" t="b">
         <v>1</v>
@@ -8580,10 +8580,10 @@
     </row>
     <row r="57" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G57" s="77" t="b">
         <v>1</v>
@@ -8597,10 +8597,10 @@
     </row>
     <row r="58" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="18" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="G58" s="77" t="b">
         <v>1</v>
@@ -8614,10 +8614,10 @@
     </row>
     <row r="59" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G59" s="77" t="b">
         <v>1</v>
@@ -8631,10 +8631,10 @@
     </row>
     <row r="60" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="G60" s="77" t="b">
         <v>1</v>
@@ -8648,10 +8648,10 @@
     </row>
     <row r="61" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G61" s="77" t="b">
         <v>1</v>
@@ -8665,10 +8665,10 @@
     </row>
     <row r="62" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="18" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="G62" s="77" t="b">
         <v>1</v>
@@ -8682,10 +8682,10 @@
     </row>
     <row r="63" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="18" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G63" s="77" t="b">
         <v>1</v>
@@ -8699,10 +8699,10 @@
     </row>
     <row r="64" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D64" s="18" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="G64" s="77" t="b">
         <v>1</v>
@@ -8716,10 +8716,10 @@
     </row>
     <row r="65" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="G65" s="77" t="b">
         <v>1</v>
@@ -8733,10 +8733,10 @@
     </row>
     <row r="66" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="G66" s="77" t="b">
         <v>1</v>
@@ -8750,10 +8750,10 @@
     </row>
     <row r="67" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="18" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="G67" s="77" t="b">
         <v>1</v>
@@ -8767,10 +8767,10 @@
     </row>
     <row r="68" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="18" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="G68" s="77" t="b">
         <v>1</v>
@@ -8784,10 +8784,10 @@
     </row>
     <row r="69" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="G69" s="77" t="b">
         <v>1</v>
@@ -8801,10 +8801,10 @@
     </row>
     <row r="70" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="18" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="G70" s="77" t="b">
         <v>1</v>
@@ -8818,10 +8818,10 @@
     </row>
     <row r="71" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="18" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="G71" s="77" t="b">
         <v>1</v>
@@ -8835,10 +8835,10 @@
     </row>
     <row r="72" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="18" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="G72" s="77" t="b">
         <v>1</v>
@@ -8852,10 +8852,10 @@
     </row>
     <row r="73" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="G73" s="77" t="b">
         <v>1</v>
@@ -8869,10 +8869,10 @@
     </row>
     <row r="74" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="18" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="G74" s="77" t="b">
         <v>1</v>
@@ -8886,10 +8886,10 @@
     </row>
     <row r="75" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="18" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="G75" s="77" t="b">
         <v>1</v>
@@ -8903,10 +8903,10 @@
     </row>
     <row r="76" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="18" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="G76" s="77" t="b">
         <v>1</v>
@@ -8920,10 +8920,10 @@
     </row>
     <row r="77" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="18" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="D77" s="18" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G77" s="77" t="b">
         <v>1</v>
@@ -8937,10 +8937,10 @@
     </row>
     <row r="78" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G78" s="77" t="b">
         <v>1</v>
@@ -8954,10 +8954,10 @@
     </row>
     <row r="79" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="G79" s="77" t="b">
         <v>1</v>
@@ -8971,10 +8971,10 @@
     </row>
     <row r="80" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="G80" s="77" t="b">
         <v>1</v>
@@ -8988,10 +8988,10 @@
     </row>
     <row r="81" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G81" s="77" t="b">
         <v>1</v>
@@ -9005,10 +9005,10 @@
     </row>
     <row r="82" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="G82" s="77" t="b">
         <v>1</v>
@@ -9022,10 +9022,10 @@
     </row>
     <row r="83" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="G83" s="77" t="b">
         <v>1</v>
@@ -9039,10 +9039,10 @@
     </row>
     <row r="84" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="18" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="G84" s="77" t="b">
         <v>1</v>
@@ -9056,10 +9056,10 @@
     </row>
     <row r="85" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="G85" s="77" t="b">
         <v>1</v>
@@ -9073,10 +9073,10 @@
     </row>
     <row r="86" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="18" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G86" s="77" t="b">
         <v>1</v>
@@ -9090,10 +9090,10 @@
     </row>
     <row r="87" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="18" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="G87" s="77" t="b">
         <v>1</v>
@@ -9107,10 +9107,10 @@
     </row>
     <row r="88" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="18" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="G88" s="77" t="b">
         <v>1</v>
@@ -9124,10 +9124,10 @@
     </row>
     <row r="89" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="18" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G89" s="77" t="b">
         <v>1</v>
@@ -9141,10 +9141,10 @@
     </row>
     <row r="90" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="18" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="G90" s="77" t="b">
         <v>1</v>
@@ -9158,10 +9158,10 @@
     </row>
     <row r="91" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D91" s="18" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="G91" s="77" t="b">
         <v>1</v>
@@ -9175,10 +9175,10 @@
     </row>
     <row r="92" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="18" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="G92" s="77" t="b">
         <v>1</v>
@@ -9192,10 +9192,10 @@
     </row>
     <row r="93" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="18" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="G93" s="77" t="b">
         <v>1</v>
@@ -9209,10 +9209,10 @@
     </row>
     <row r="94" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="18" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="G94" s="77" t="b">
         <v>1</v>
@@ -9226,10 +9226,10 @@
     </row>
     <row r="95" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="18" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="D95" s="18" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G95" s="77" t="b">
         <v>1</v>
@@ -9243,10 +9243,10 @@
     </row>
     <row r="96" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="18" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="G96" s="77" t="b">
         <v>1</v>
@@ -9260,10 +9260,10 @@
     </row>
     <row r="97" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="18" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="D97" s="18" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="G97" s="77" t="b">
         <v>1</v>
@@ -9277,10 +9277,10 @@
     </row>
     <row r="98" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="18" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="G98" s="77" t="b">
         <v>1</v>
@@ -9294,10 +9294,10 @@
     </row>
     <row r="99" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="18" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G99" s="77" t="b">
         <v>1</v>
@@ -9311,10 +9311,10 @@
     </row>
     <row r="100" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="18" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="G100" s="77" t="b">
         <v>1</v>
@@ -9328,10 +9328,10 @@
     </row>
     <row r="101" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="18" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="D101" s="18" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G101" s="77" t="b">
         <v>1</v>
@@ -9345,10 +9345,10 @@
     </row>
     <row r="102" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="18" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="G102" s="77" t="b">
         <v>1</v>
@@ -9362,10 +9362,10 @@
     </row>
     <row r="103" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="18" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="G103" s="77" t="b">
         <v>1</v>
@@ -9379,10 +9379,10 @@
     </row>
     <row r="104" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="18" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="G104" s="77" t="b">
         <v>1</v>
@@ -9396,10 +9396,10 @@
     </row>
     <row r="105" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="18" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G105" s="77" t="b">
         <v>1</v>
@@ -9413,10 +9413,10 @@
     </row>
     <row r="106" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="18" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="G106" s="77" t="b">
         <v>1</v>
@@ -9430,10 +9430,10 @@
     </row>
     <row r="107" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="18" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="G107" s="77" t="b">
         <v>1</v>
@@ -9447,10 +9447,10 @@
     </row>
     <row r="108" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="G108" s="77" t="b">
         <v>1</v>
@@ -9464,10 +9464,10 @@
     </row>
     <row r="109" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="D109" s="18" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G109" s="77" t="b">
         <v>1</v>
@@ -9481,10 +9481,10 @@
     </row>
     <row r="110" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="G110" s="77" t="b">
         <v>1</v>
@@ -9498,10 +9498,10 @@
     </row>
     <row r="111" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="D111" s="18" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G111" s="77" t="b">
         <v>1</v>
@@ -9515,10 +9515,10 @@
     </row>
     <row r="112" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="D112" s="18" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G112" s="77" t="b">
         <v>1</v>
@@ -9532,10 +9532,10 @@
     </row>
     <row r="113" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="G113" s="77" t="b">
         <v>1</v>
@@ -9549,10 +9549,10 @@
     </row>
     <row r="114" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="G114" s="77" t="b">
         <v>1</v>
@@ -9566,10 +9566,10 @@
     </row>
     <row r="115" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="D115" s="18" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="G115" s="77" t="b">
         <v>1</v>
@@ -9583,10 +9583,10 @@
     </row>
     <row r="116" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="D116" s="18" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="G116" s="77" t="b">
         <v>1</v>
@@ -9600,10 +9600,10 @@
     </row>
     <row r="117" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="D117" s="18" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="G117" s="77" t="b">
         <v>1</v>
@@ -9617,10 +9617,10 @@
     </row>
     <row r="118" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="D118" s="18" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="G118" s="77" t="b">
         <v>1</v>
@@ -9634,10 +9634,10 @@
     </row>
     <row r="119" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="D119" s="18" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="G119" s="77" t="b">
         <v>1</v>
@@ -9651,10 +9651,10 @@
     </row>
     <row r="120" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A120" s="18" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="D120" s="18" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G120" s="77" t="b">
         <v>1</v>
@@ -9668,10 +9668,10 @@
     </row>
     <row r="121" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A121" s="18" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="D121" s="18" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="G121" s="77" t="b">
         <v>1</v>
@@ -9685,10 +9685,10 @@
     </row>
     <row r="122" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="D122" s="18" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="G122" s="77" t="b">
         <v>1</v>
@@ -9702,10 +9702,10 @@
     </row>
     <row r="123" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123" s="18" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="D123" s="18" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="G123" s="77" t="b">
         <v>1</v>
@@ -9719,10 +9719,10 @@
     </row>
     <row r="124" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="18" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="G124" s="77" t="b">
         <v>1</v>
@@ -9736,10 +9736,10 @@
     </row>
     <row r="125" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="18" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="G125" s="77" t="b">
         <v>1</v>
@@ -9753,10 +9753,10 @@
     </row>
     <row r="126" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A126" s="18" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="G126" s="77" t="b">
         <v>1</v>
@@ -9770,10 +9770,10 @@
     </row>
     <row r="127" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A127" s="18" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="G127" s="77" t="b">
         <v>1</v>
@@ -9787,10 +9787,10 @@
     </row>
     <row r="128" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="18" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="G128" s="77" t="b">
         <v>1</v>
@@ -9804,10 +9804,10 @@
     </row>
     <row r="129" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A129" s="18" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="D129" s="18" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="G129" s="77" t="b">
         <v>1</v>
@@ -9821,10 +9821,10 @@
     </row>
     <row r="130" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="18" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D130" s="18" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="G130" s="77" t="b">
         <v>1</v>
@@ -9838,10 +9838,10 @@
     </row>
     <row r="131" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="18" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D131" s="18" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="G131" s="77" t="b">
         <v>1</v>
@@ -9855,10 +9855,10 @@
     </row>
     <row r="132" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="18" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="G132" s="77" t="b">
         <v>1</v>
@@ -9872,10 +9872,10 @@
     </row>
     <row r="133" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="18" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="D133" s="18" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="G133" s="77" t="b">
         <v>1</v>
@@ -9889,10 +9889,10 @@
     </row>
     <row r="134" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="18" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D134" s="18" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="G134" s="77" t="b">
         <v>1</v>
@@ -9906,10 +9906,10 @@
     </row>
     <row r="135" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="18" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="D135" s="18" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="G135" s="77" t="b">
         <v>1</v>
@@ -9923,10 +9923,10 @@
     </row>
     <row r="136" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="18" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="G136" s="77" t="b">
         <v>1</v>
@@ -9940,10 +9940,10 @@
     </row>
     <row r="137" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A137" s="18" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D137" s="18" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="G137" s="77" t="b">
         <v>1</v>
@@ -9957,10 +9957,10 @@
     </row>
     <row r="138" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A138" s="18" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="D138" s="18" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="G138" s="77" t="b">
         <v>1</v>
@@ -9974,10 +9974,10 @@
     </row>
     <row r="139" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A139" s="18" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D139" s="18" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G139" s="77" t="b">
         <v>1</v>
@@ -9991,10 +9991,10 @@
     </row>
     <row r="140" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A140" s="18" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="D140" s="18" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="G140" s="77" t="b">
         <v>1</v>
@@ -10008,10 +10008,10 @@
     </row>
     <row r="141" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A141" s="18" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D141" s="18" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G141" s="77" t="b">
         <v>1</v>
@@ -10025,10 +10025,10 @@
     </row>
     <row r="142" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A142" s="18" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D142" s="18" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="G142" s="77" t="b">
         <v>1</v>
@@ -10042,10 +10042,10 @@
     </row>
     <row r="143" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A143" s="18" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="D143" s="18" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G143" s="77" t="b">
         <v>1</v>
@@ -10059,10 +10059,10 @@
     </row>
     <row r="144" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A144" s="18" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="D144" s="18" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="G144" s="77" t="b">
         <v>1</v>
@@ -10076,10 +10076,10 @@
     </row>
     <row r="145" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="18" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="D145" s="18" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G145" s="77" t="b">
         <v>1</v>
@@ -10093,10 +10093,10 @@
     </row>
     <row r="146" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A146" s="18" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="D146" s="18" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="G146" s="77" t="b">
         <v>1</v>
@@ -10110,10 +10110,10 @@
     </row>
     <row r="147" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="18" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="D147" s="18" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="G147" s="77" t="b">
         <v>1</v>
@@ -10127,10 +10127,10 @@
     </row>
     <row r="148" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="18" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="D148" s="18" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="G148" s="77" t="b">
         <v>1</v>
@@ -10144,10 +10144,10 @@
     </row>
     <row r="149" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="18" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="D149" s="18" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="G149" s="77" t="b">
         <v>1</v>
@@ -10161,10 +10161,10 @@
     </row>
     <row r="150" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="18" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="D150" s="18" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="G150" s="77" t="b">
         <v>1</v>
@@ -10178,10 +10178,10 @@
     </row>
     <row r="151" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="18" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D151" s="18" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="G151" s="77" t="b">
         <v>1</v>
@@ -10195,10 +10195,10 @@
     </row>
     <row r="152" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A152" s="18" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D152" s="18" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="G152" s="77" t="b">
         <v>1</v>
@@ -10212,10 +10212,10 @@
     </row>
     <row r="153" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A153" s="18" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="D153" s="18" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="G153" s="77" t="b">
         <v>1</v>
@@ -10229,10 +10229,10 @@
     </row>
     <row r="154" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="18" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D154" s="18" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="G154" s="77" t="b">
         <v>1</v>
@@ -10246,10 +10246,10 @@
     </row>
     <row r="155" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A155" s="18" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="D155" s="18" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="G155" s="77" t="b">
         <v>1</v>
@@ -10263,10 +10263,10 @@
     </row>
     <row r="156" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A156" s="18" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="D156" s="18" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="G156" s="77" t="b">
         <v>1</v>
@@ -10280,10 +10280,10 @@
     </row>
     <row r="157" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A157" s="18" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="D157" s="18" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="G157" s="77" t="b">
         <v>1</v>
@@ -10297,10 +10297,10 @@
     </row>
     <row r="158" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A158" s="18" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="D158" s="18" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="G158" s="77" t="b">
         <v>1</v>
@@ -10314,10 +10314,10 @@
     </row>
     <row r="159" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A159" s="18" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D159" s="18" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="G159" s="77" t="b">
         <v>1</v>
@@ -10331,10 +10331,10 @@
     </row>
     <row r="160" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="18" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="D160" s="18" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="G160" s="77" t="b">
         <v>1</v>
@@ -10348,10 +10348,10 @@
     </row>
     <row r="161" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A161" s="18" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D161" s="18" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G161" s="77" t="b">
         <v>1</v>
@@ -10365,10 +10365,10 @@
     </row>
     <row r="162" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A162" s="18" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D162" s="18" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="G162" s="77" t="b">
         <v>1</v>
@@ -10382,10 +10382,10 @@
     </row>
     <row r="163" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A163" s="18" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D163" s="18" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G163" s="77" t="b">
         <v>1</v>
@@ -10399,10 +10399,10 @@
     </row>
     <row r="164" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A164" s="18" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D164" s="18" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="G164" s="77" t="b">
         <v>1</v>
@@ -10416,10 +10416,10 @@
     </row>
     <row r="165" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="18" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D165" s="18" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G165" s="77" t="b">
         <v>1</v>
@@ -10433,10 +10433,10 @@
     </row>
     <row r="166" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A166" s="18" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="D166" s="18" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G166" s="77" t="b">
         <v>1</v>
@@ -10450,10 +10450,10 @@
     </row>
     <row r="167" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="18" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D167" s="18" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="G167" s="77" t="b">
         <v>1</v>
@@ -10467,10 +10467,10 @@
     </row>
     <row r="168" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A168" s="18" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="D168" s="18" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="G168" s="77" t="b">
         <v>1</v>
@@ -10484,10 +10484,10 @@
     </row>
     <row r="169" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A169" s="18" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="D169" s="18" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="G169" s="77" t="b">
         <v>1</v>
@@ -10501,10 +10501,10 @@
     </row>
     <row r="170" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A170" s="18" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="D170" s="18" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G170" s="77" t="b">
         <v>1</v>
@@ -10518,10 +10518,10 @@
     </row>
     <row r="171" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="18" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="D171" s="18" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="G171" s="77" t="b">
         <v>1</v>
@@ -10535,10 +10535,10 @@
     </row>
     <row r="172" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A172" s="18" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="D172" s="18" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="G172" s="77" t="b">
         <v>1</v>
@@ -10552,10 +10552,10 @@
     </row>
     <row r="173" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A173" s="18" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="D173" s="18" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="G173" s="77" t="b">
         <v>1</v>
@@ -10569,10 +10569,10 @@
     </row>
     <row r="174" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="18" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="D174" s="18" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="G174" s="77" t="b">
         <v>1</v>
@@ -10586,10 +10586,10 @@
     </row>
     <row r="175" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A175" s="18" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D175" s="18" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G175" s="77" t="b">
         <v>1</v>
@@ -10603,10 +10603,10 @@
     </row>
     <row r="176" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A176" s="18" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="D176" s="18" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="G176" s="77" t="b">
         <v>1</v>
@@ -10620,10 +10620,10 @@
     </row>
     <row r="177" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A177" s="18" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="D177" s="18" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="G177" s="77" t="b">
         <v>1</v>
@@ -10637,10 +10637,10 @@
     </row>
     <row r="178" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A178" s="18" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="D178" s="18" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="G178" s="77" t="b">
         <v>1</v>
@@ -10654,10 +10654,10 @@
     </row>
     <row r="179" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A179" s="18" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="D179" s="18" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="G179" s="77" t="b">
         <v>1</v>
@@ -10671,10 +10671,10 @@
     </row>
     <row r="180" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="18" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D180" s="18" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G180" s="77" t="b">
         <v>1</v>
@@ -10688,10 +10688,10 @@
     </row>
     <row r="181" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A181" s="18" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D181" s="18" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="G181" s="77" t="b">
         <v>1</v>
@@ -10705,10 +10705,10 @@
     </row>
     <row r="182" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A182" s="18" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D182" s="18" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="G182" s="77" t="b">
         <v>1</v>
@@ -10722,10 +10722,10 @@
     </row>
     <row r="183" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A183" s="18" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="D183" s="18" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="G183" s="77" t="b">
         <v>1</v>
@@ -10739,10 +10739,10 @@
     </row>
     <row r="184" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A184" s="18" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="D184" s="18" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="G184" s="77" t="b">
         <v>1</v>
@@ -10756,10 +10756,10 @@
     </row>
     <row r="185" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A185" s="18" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D185" s="18" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="G185" s="77" t="b">
         <v>1</v>
@@ -10773,10 +10773,10 @@
     </row>
     <row r="186" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A186" s="18" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="D186" s="18" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="G186" s="77" t="b">
         <v>1</v>
@@ -10790,10 +10790,10 @@
     </row>
     <row r="187" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A187" s="18" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="D187" s="18" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G187" s="77" t="b">
         <v>1</v>
@@ -10807,10 +10807,10 @@
     </row>
     <row r="188" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A188" s="18" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D188" s="18" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="G188" s="77" t="b">
         <v>1</v>
@@ -10824,10 +10824,10 @@
     </row>
     <row r="189" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A189" s="18" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D189" s="18" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G189" s="77" t="b">
         <v>1</v>
@@ -10841,10 +10841,10 @@
     </row>
     <row r="190" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A190" s="18" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="D190" s="18" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="G190" s="77" t="b">
         <v>1</v>
@@ -10858,10 +10858,10 @@
     </row>
     <row r="191" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="18" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="D191" s="18" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="G191" s="77" t="b">
         <v>1</v>
@@ -10875,10 +10875,10 @@
     </row>
     <row r="192" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A192" s="18" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="D192" s="18" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G192" s="77" t="b">
         <v>1</v>
@@ -10892,10 +10892,10 @@
     </row>
     <row r="193" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A193" s="18" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="D193" s="18" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="G193" s="77" t="b">
         <v>1</v>
@@ -10909,10 +10909,10 @@
     </row>
     <row r="194" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A194" s="18" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="D194" s="18" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="G194" s="77" t="b">
         <v>1</v>
@@ -10926,10 +10926,10 @@
     </row>
     <row r="195" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A195" s="18" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="D195" s="18" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="G195" s="77" t="b">
         <v>1</v>
@@ -10943,10 +10943,10 @@
     </row>
     <row r="196" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A196" s="18" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D196" s="18" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="G196" s="77" t="b">
         <v>1</v>
@@ -10960,10 +10960,10 @@
     </row>
     <row r="197" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A197" s="18" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D197" s="18" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="G197" s="77" t="b">
         <v>1</v>
@@ -11492,14 +11492,14 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="60.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
@@ -11510,7 +11510,7 @@
     <col min="18" max="18" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="44" customFormat="1" ht="14.45" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="44" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="b">
         <v>1</v>
       </c>
@@ -11529,7 +11529,7 @@
       <c r="H1" s="45"/>
       <c r="I1" s="45"/>
     </row>
-    <row r="2" spans="1:18" s="29" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="29" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B2" s="46" t="s">
         <v>221</v>
       </c>
@@ -11543,31 +11543,31 @@
         <v>209</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="L2" s="29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N2" s="29" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="P2" s="29" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="R2" s="29" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:18" s="29" customFormat="1" ht="14.45" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="29" customFormat="1" ht="14.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B3" s="46" t="s">
         <v>221</v>
       </c>
@@ -11581,31 +11581,31 @@
         <v>209</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="J3" s="29" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="N3" s="29" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="P3" s="29" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="R3" s="29" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="29" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="29" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B4" s="46" t="s">
         <v>221</v>
       </c>
@@ -11619,77 +11619,77 @@
         <v>209</v>
       </c>
       <c r="I4" s="43" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="K4" s="43" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L4" s="43" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="M4" s="43" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="N4" s="43" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="P4" s="43" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="R4" s="29" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:18" s="29" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="29" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="B5" s="46" t="s">
         <v>221</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="G5" s="29" t="s">
         <v>209</v>
       </c>
       <c r="I5" s="43" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="K5" s="43" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="L5" s="43" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M5" s="43" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N5" s="43" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="P5" s="43" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="R5" s="29" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="47" customFormat="1" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="b">
         <v>0</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D9" s="50" t="s">
         <v>45</v>
@@ -11700,19 +11700,19 @@
       <c r="H9" s="50"/>
       <c r="I9" s="50"/>
     </row>
-    <row r="10" spans="1:18" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50"/>
       <c r="B10" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E10" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F10" s="50" t="s">
         <v>43</v>
@@ -11723,19 +11723,19 @@
       </c>
       <c r="I10" s="50"/>
     </row>
-    <row r="11" spans="1:18" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="50"/>
       <c r="B11" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="50" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E11" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F11" s="50" t="s">
         <v>43</v>
@@ -11746,19 +11746,19 @@
       </c>
       <c r="I11" s="50"/>
     </row>
-    <row r="12" spans="1:18" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="50"/>
       <c r="B12" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="50" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D12" s="50" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E12" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F12" s="50" t="s">
         <v>43</v>
@@ -11769,19 +11769,19 @@
       </c>
       <c r="I12" s="50"/>
     </row>
-    <row r="13" spans="1:18" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="50"/>
       <c r="B13" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="50" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D13" s="50" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F13" s="50" t="s">
         <v>44</v>
@@ -11792,15 +11792,15 @@
       </c>
       <c r="I13" s="50"/>
     </row>
-    <row r="14" spans="1:18" s="47" customFormat="1" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="50" t="b">
         <v>0</v>
       </c>
       <c r="B14" s="50" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C14" s="50" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D14" s="50" t="s">
         <v>45</v>
@@ -11811,19 +11811,19 @@
       <c r="H14" s="50"/>
       <c r="I14" s="50"/>
     </row>
-    <row r="15" spans="1:18" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="50"/>
       <c r="B15" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="50" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D15" s="50" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E15" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F15" s="50" t="s">
         <v>43</v>
@@ -11834,19 +11834,19 @@
       </c>
       <c r="I15" s="50"/>
     </row>
-    <row r="16" spans="1:18" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50"/>
       <c r="B16" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="50" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D16" s="50" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="E16" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F16" s="50" t="s">
         <v>43</v>
@@ -11857,19 +11857,19 @@
       </c>
       <c r="I16" s="50"/>
     </row>
-    <row r="17" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50"/>
       <c r="B17" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="50" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="E17" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F17" s="50" t="s">
         <v>43</v>
@@ -11880,19 +11880,19 @@
       </c>
       <c r="I17" s="50"/>
     </row>
-    <row r="18" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50"/>
       <c r="B18" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="50" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D18" s="50" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="E18" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F18" s="50" t="s">
         <v>44</v>
@@ -11903,15 +11903,15 @@
       </c>
       <c r="I18" s="50"/>
     </row>
-    <row r="19" spans="1:9" s="47" customFormat="1" ht="15.75" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="47" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="b">
         <v>0</v>
       </c>
       <c r="B19" s="50" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C19" s="50" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D19" s="50" t="s">
         <v>45</v>
@@ -11922,44 +11922,44 @@
       <c r="H19" s="50"/>
       <c r="I19" s="50"/>
     </row>
-    <row r="20" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50"/>
       <c r="B20" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="50" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D20" s="50" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E20" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F20" s="50" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="G20" s="50"/>
       <c r="H20" s="50" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I20" s="50" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="50"/>
       <c r="B21" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C21" s="50" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D21" s="50" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E21" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F21" s="50" t="s">
         <v>43</v>
@@ -11970,19 +11970,19 @@
       </c>
       <c r="I21" s="50"/>
     </row>
-    <row r="22" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="50"/>
       <c r="B22" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="50" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D22" s="50" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E22" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F22" s="50" t="s">
         <v>43</v>
@@ -11993,19 +11993,19 @@
       </c>
       <c r="I22" s="50"/>
     </row>
-    <row r="23" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="50"/>
       <c r="B23" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="50" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D23" s="50" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="E23" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F23" s="50" t="s">
         <v>43</v>
@@ -12016,19 +12016,19 @@
       </c>
       <c r="I23" s="50"/>
     </row>
-    <row r="24" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="50"/>
       <c r="B24" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="50" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D24" s="50" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="E24" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F24" s="50" t="s">
         <v>44</v>
@@ -12039,19 +12039,19 @@
       </c>
       <c r="I24" s="50"/>
     </row>
-    <row r="25" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="50"/>
       <c r="B25" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C25" s="50" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="D25" s="50" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E25" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F25" s="50" t="s">
         <v>42</v>
@@ -12062,19 +12062,19 @@
       </c>
       <c r="I25" s="50"/>
     </row>
-    <row r="26" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50"/>
       <c r="B26" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C26" s="50" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D26" s="50" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F26" s="50" t="s">
         <v>44</v>
@@ -12085,19 +12085,19 @@
       </c>
       <c r="I26" s="50"/>
     </row>
-    <row r="27" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="50"/>
       <c r="B27" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="D27" s="50" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E27" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F27" s="50" t="s">
         <v>43</v>
@@ -12108,19 +12108,19 @@
       </c>
       <c r="I27" s="50"/>
     </row>
-    <row r="28" spans="1:9" s="47" customFormat="1" ht="15.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" s="47" customFormat="1" ht="15.75" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="50"/>
       <c r="B28" s="50" t="s">
         <v>20</v>
       </c>
       <c r="C28" s="50" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="D28" s="50" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="F28" s="50" t="s">
         <v>44</v>
@@ -12136,10 +12136,10 @@
         <v>0</v>
       </c>
       <c r="B29" s="50" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D29" s="50" t="s">
         <v>45</v>

</xml_diff>